<commit_message>
code style improvements on the enrichment calculator function
</commit_message>
<xml_diff>
--- a/src/GCModeller/annotations/GSEA/data/TCS_result_KO.xlsx
+++ b/src/GCModeller/annotations/GSEA/data/TCS_result_KO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GCModeller\src\GCModeller\annotations\GSEA\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="23715" windowHeight="10755"/>
   </bookViews>
@@ -778,12 +783,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -791,7 +796,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -800,7 +805,7 @@
       <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Cambria"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="major"/>
@@ -809,7 +814,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -818,7 +823,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -827,7 +832,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -835,7 +840,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -843,7 +848,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -851,7 +856,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -859,7 +864,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -868,7 +873,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -877,7 +882,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -885,7 +890,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -894,7 +899,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -902,7 +907,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -911,7 +916,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -920,7 +925,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -928,16 +933,24 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1372,7 +1385,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1380,52 +1393,58 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - 强调文字颜色 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="标题 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="标题 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="差" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="汇总" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="计算" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="检查单元格" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="解释性文本" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1433,12 +1452,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1480,7 +1502,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1515,7 +1537,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1727,25 +1749,25 @@
   <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.5" customWidth="1"/>
-    <col min="3" max="3" width="50.125" customWidth="1"/>
-    <col min="4" max="6" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -1770,11 +1792,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1799,11 +1821,11 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>125</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1828,11 +1850,11 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" s="1" customFormat="1">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1857,11 +1879,11 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" s="1" customFormat="1">
       <c r="A5" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>201</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -1886,11 +1908,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" s="1" customFormat="1">
       <c r="A6" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>207</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1915,11 +1937,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" s="1" customFormat="1">
       <c r="A7" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="4" t="s">
         <v>130</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1944,11 +1966,11 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" s="1" customFormat="1">
       <c r="A8" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="4" t="s">
         <v>204</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1973,11 +1995,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" s="1" customFormat="1">
       <c r="A9" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="4" t="s">
         <v>145</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -2002,11 +2024,11 @@
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" s="1" customFormat="1">
       <c r="A10" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="4" t="s">
         <v>121</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -2031,11 +2053,11 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" s="1" customFormat="1">
       <c r="A11" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="4" t="s">
         <v>53</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -2060,11 +2082,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" s="1" customFormat="1">
       <c r="A12" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="4" t="s">
         <v>195</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -2089,11 +2111,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" s="1" customFormat="1">
       <c r="A13" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="4" t="s">
         <v>198</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -2118,11 +2140,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" s="1" customFormat="1">
       <c r="A14" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="4" t="s">
         <v>210</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -2147,11 +2169,11 @@
         <v>212</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" s="1" customFormat="1">
       <c r="A15" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="4" t="s">
         <v>134</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -2176,11 +2198,11 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" s="1" customFormat="1">
       <c r="A16" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -2205,11 +2227,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" s="1" customFormat="1">
       <c r="A17" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="4" t="s">
         <v>141</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -2234,11 +2256,11 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" s="1" customFormat="1">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -2263,11 +2285,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" s="1" customFormat="1">
       <c r="A19" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="4" t="s">
         <v>113</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -2292,11 +2314,11 @@
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" s="1" customFormat="1">
       <c r="A20" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="4" t="s">
         <v>149</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -2321,11 +2343,11 @@
         <v>151</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" s="1" customFormat="1">
       <c r="A21" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="4" t="s">
         <v>156</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -2350,11 +2372,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" s="1" customFormat="1">
       <c r="A22" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="4" t="s">
         <v>186</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -2379,11 +2401,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" s="1" customFormat="1">
       <c r="A23" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -2408,11 +2430,11 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" s="1" customFormat="1">
       <c r="A24" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="4" t="s">
         <v>168</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -2437,11 +2459,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9" s="1" customFormat="1">
       <c r="A25" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="4" t="s">
         <v>84</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -2466,11 +2488,11 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9" s="1" customFormat="1">
       <c r="A26" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="4" t="s">
         <v>105</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -2495,11 +2517,11 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9" s="1" customFormat="1">
       <c r="A27" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -2524,11 +2546,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9" s="1" customFormat="1">
       <c r="A28" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -2553,11 +2575,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>179</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="3" t="s">
         <v>180</v>
       </c>
       <c r="C29" t="s">
@@ -2582,11 +2604,11 @@
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>213</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="3" t="s">
         <v>214</v>
       </c>
       <c r="C30" t="s">
@@ -2611,11 +2633,11 @@
         <v>216</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>217</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="3" t="s">
         <v>218</v>
       </c>
       <c r="C31" t="s">
@@ -2640,11 +2662,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>220</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="3" t="s">
         <v>221</v>
       </c>
       <c r="C32" t="s">
@@ -2669,11 +2691,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
         <v>223</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="3" t="s">
         <v>224</v>
       </c>
       <c r="C33" t="s">
@@ -2698,11 +2720,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>226</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="3" t="s">
         <v>227</v>
       </c>
       <c r="C34" t="s">
@@ -2727,11 +2749,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>229</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="3" t="s">
         <v>230</v>
       </c>
       <c r="C35" t="s">
@@ -2756,11 +2778,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
         <v>232</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="3" t="s">
         <v>233</v>
       </c>
       <c r="C36" t="s">
@@ -2785,11 +2807,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
         <v>235</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="3" t="s">
         <v>236</v>
       </c>
       <c r="C37" t="s">
@@ -2814,11 +2836,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
         <v>238</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="3" t="s">
         <v>239</v>
       </c>
       <c r="C38" t="s">
@@ -2843,11 +2865,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
         <v>241</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="3" t="s">
         <v>242</v>
       </c>
       <c r="C39" t="s">
@@ -2872,11 +2894,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:9">
       <c r="A40" t="s">
         <v>244</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="3" t="s">
         <v>245</v>
       </c>
       <c r="C40" t="s">
@@ -2901,11 +2923,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
         <v>247</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="3" t="s">
         <v>248</v>
       </c>
       <c r="C41" t="s">
@@ -2930,11 +2952,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
         <v>250</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="3" t="s">
         <v>251</v>
       </c>
       <c r="C42" t="s">
@@ -2959,11 +2981,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
         <v>176</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="3" t="s">
         <v>177</v>
       </c>
       <c r="C43" t="s">
@@ -2988,11 +3010,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
         <v>117</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="3" t="s">
         <v>118</v>
       </c>
       <c r="C44" t="s">
@@ -3017,11 +3039,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
         <v>43</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="3" t="s">
         <v>44</v>
       </c>
       <c r="C45" t="s">
@@ -3046,11 +3068,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:9">
       <c r="A46" t="s">
         <v>75</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C46" t="s">
@@ -3075,11 +3097,11 @@
         <v>78</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:9">
       <c r="A47" t="s">
         <v>188</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="3" t="s">
         <v>189</v>
       </c>
       <c r="C47" t="s">
@@ -3104,11 +3126,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:9">
       <c r="A48" t="s">
         <v>87</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="3" t="s">
         <v>88</v>
       </c>
       <c r="C48" t="s">
@@ -3133,11 +3155,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
         <v>56</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="3" t="s">
         <v>57</v>
       </c>
       <c r="C49" t="s">
@@ -3162,11 +3184,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:9">
       <c r="A50" t="s">
         <v>164</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="3" t="s">
         <v>165</v>
       </c>
       <c r="C50" t="s">
@@ -3191,11 +3213,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:9">
       <c r="A51" t="s">
         <v>182</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="3" t="s">
         <v>183</v>
       </c>
       <c r="C51" t="s">
@@ -3220,11 +3242,11 @@
         <v>38</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:9">
       <c r="A52" t="s">
         <v>191</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="3" t="s">
         <v>192</v>
       </c>
       <c r="C52" t="s">
@@ -3249,11 +3271,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:9">
       <c r="A53" t="s">
         <v>158</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C53" t="s">
@@ -3278,11 +3300,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:9">
       <c r="A54" t="s">
         <v>60</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C54" t="s">
@@ -3307,11 +3329,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:9">
       <c r="A55" t="s">
         <v>152</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="3" t="s">
         <v>153</v>
       </c>
       <c r="C55" t="s">
@@ -3336,11 +3358,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:9">
       <c r="A56" t="s">
         <v>9</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C56" t="s">
@@ -3365,11 +3387,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:9">
       <c r="A57" t="s">
         <v>137</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="3" t="s">
         <v>138</v>
       </c>
       <c r="C57" t="s">
@@ -3394,11 +3416,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:9">
       <c r="A58" t="s">
         <v>161</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="3" t="s">
         <v>162</v>
       </c>
       <c r="C58" t="s">
@@ -3423,11 +3445,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:9">
       <c r="A59" t="s">
         <v>108</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="3" t="s">
         <v>109</v>
       </c>
       <c r="C59" t="s">
@@ -3452,11 +3474,11 @@
         <v>111</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:9">
       <c r="A60" t="s">
         <v>94</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="3" t="s">
         <v>95</v>
       </c>
       <c r="C60" t="s">
@@ -3481,11 +3503,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:9">
       <c r="A61" t="s">
         <v>39</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C61" t="s">
@@ -3510,11 +3532,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:9">
       <c r="A62" t="s">
         <v>170</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="3" t="s">
         <v>171</v>
       </c>
       <c r="C62" t="s">
@@ -3539,11 +3561,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:9">
       <c r="A63" t="s">
         <v>63</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C63" t="s">
@@ -3568,11 +3590,11 @@
         <v>66</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:9">
       <c r="A64" t="s">
         <v>67</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C64" t="s">
@@ -3597,11 +3619,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:9">
       <c r="A65" t="s">
         <v>79</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="3" t="s">
         <v>80</v>
       </c>
       <c r="C65" t="s">
@@ -3626,11 +3648,11 @@
         <v>82</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:9">
       <c r="A66" t="s">
         <v>34</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C66" t="s">
@@ -3655,11 +3677,11 @@
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:9">
       <c r="A67" t="s">
         <v>100</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="3" t="s">
         <v>101</v>
       </c>
       <c r="C67" t="s">
@@ -3684,11 +3706,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:9">
       <c r="A68" t="s">
         <v>71</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="3" t="s">
         <v>72</v>
       </c>
       <c r="C68" t="s">
@@ -3713,11 +3735,11 @@
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:9">
       <c r="A69" t="s">
         <v>48</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C69" t="s">
@@ -3760,5 +3782,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>